<commit_message>
Modification in the dashboard
</commit_message>
<xml_diff>
--- a/Interactive Dashboard.xlsx
+++ b/Interactive Dashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minaf\Desktop\Excel\Kevin The Analyst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minaf\Desktop\Excel\Kevin The Analyst\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB743C06-8729-4792-8E2A-3C0CF2507104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D735D659-C686-4596-A3FF-239F008C3257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74C88240-846C-43E5-B6B7-237F75EF3103}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -682,7 +682,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Profite by Market &amp; Cookie Type</a:t>
+              <a:t>Profit by Market &amp; Cookie Type</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1295,19 +1295,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>81522</c:v>
+                  <c:v>99915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70356</c:v>
+                  <c:v>86598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67500</c:v>
+                  <c:v>81960</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72831</c:v>
+                  <c:v>80013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49086</c:v>
+                  <c:v>60726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,19 +1372,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34414.25</c:v>
+                  <c:v>46744.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29061.5</c:v>
+                  <c:v>36530</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43858.75</c:v>
+                  <c:v>51853.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23029.5</c:v>
+                  <c:v>27563.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37719.5</c:v>
+                  <c:v>41967.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,19 +1449,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>23228.799999999999</c:v>
+                  <c:v>27795.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34554.799999999996</c:v>
+                  <c:v>44136.400000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32177.599999999999</c:v>
+                  <c:v>41137.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23083.200000000004</c:v>
+                  <c:v>27795.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23615.199999999997</c:v>
+                  <c:v>28335.999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1526,19 +1526,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34902.5</c:v>
+                  <c:v>36950</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>33997.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14577.5</c:v>
+                  <c:v>20900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25822.5</c:v>
+                  <c:v>27825</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26897.5</c:v>
+                  <c:v>33925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,19 +1603,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27520.5</c:v>
+                  <c:v>29036</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18305</c:v>
+                  <c:v>25086.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27972</c:v>
+                  <c:v>28736.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15384.25</c:v>
+                  <c:v>16506</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14320.25</c:v>
+                  <c:v>15181.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,19 +1680,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8657.5999999999985</c:v>
+                  <c:v>10790.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9571.2000000000007</c:v>
+                  <c:v>10672</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8023.2</c:v>
+                  <c:v>10924.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7951.9999999999991</c:v>
+                  <c:v>9755.9999999999982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8628</c:v>
+                  <c:v>9144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2468,7 +2468,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Profite by month</a:t>
+              <a:t>Profit by month</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3400,19 +3400,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>81522</c:v>
+                  <c:v>99915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70356</c:v>
+                  <c:v>86598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67500</c:v>
+                  <c:v>81960</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72831</c:v>
+                  <c:v>80013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49086</c:v>
+                  <c:v>60726</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3477,19 +3477,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34414.25</c:v>
+                  <c:v>46744.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29061.5</c:v>
+                  <c:v>36530</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43858.75</c:v>
+                  <c:v>51853.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23029.5</c:v>
+                  <c:v>27563.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37719.5</c:v>
+                  <c:v>41967.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3554,19 +3554,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>23228.799999999999</c:v>
+                  <c:v>27795.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34554.799999999996</c:v>
+                  <c:v>44136.400000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32177.599999999999</c:v>
+                  <c:v>41137.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23083.200000000004</c:v>
+                  <c:v>27795.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23615.199999999997</c:v>
+                  <c:v>28335.999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3631,19 +3631,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>34902.5</c:v>
+                  <c:v>36950</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>33997.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14577.5</c:v>
+                  <c:v>20900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25822.5</c:v>
+                  <c:v>27825</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26897.5</c:v>
+                  <c:v>33925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3708,19 +3708,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27520.5</c:v>
+                  <c:v>29036</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18305</c:v>
+                  <c:v>25086.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27972</c:v>
+                  <c:v>28736.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15384.25</c:v>
+                  <c:v>16506</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14320.25</c:v>
+                  <c:v>15181.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3785,19 +3785,19 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8657.5999999999985</c:v>
+                  <c:v>10790.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9571.2000000000007</c:v>
+                  <c:v>10672</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8023.2</c:v>
+                  <c:v>10924.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7951.9999999999991</c:v>
+                  <c:v>9755.9999999999982</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8628</c:v>
+                  <c:v>9144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15179,7 +15179,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19940CEB-5EF1-4D0C-B264-8D97B1710E23}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{19940CEB-5EF1-4D0C-B264-8D97B1710E23}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:H10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -15470,11 +15470,11 @@
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="6" type="dateBetween" evalOrder="-1" id="17" name="Date">
+    <filter fld="6" type="dateBetween" evalOrder="-1" id="19" name="Date">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <customFilters and="1">
-            <customFilter operator="greaterThanOrEqual" val="44044"/>
+            <customFilter operator="greaterThanOrEqual" val="44013"/>
             <customFilter operator="lessThanOrEqual" val="44196"/>
           </customFilters>
         </filterColumn>
@@ -15498,7 +15498,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B78E44B9-1145-4825-AB5C-AA7E904E8B90}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B78E44B9-1145-4825-AB5C-AA7E904E8B90}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -15644,7 +15644,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD17A3B6-1A77-47E6-BC1A-ED7B30761FA4}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD17A3B6-1A77-47E6-BC1A-ED7B30761FA4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -16115,7 +16115,7 @@
     <pivotTable tabId="4" name="PivotTable1"/>
   </pivotTables>
   <state minimalRefreshVersion="6" lastRefreshVersion="6" pivotCacheId="292933435" filterType="dateBetween">
-    <selection startDate="2020-08-01T00:00:00" endDate="2020-12-31T00:00:00"/>
+    <selection startDate="2020-07-01T00:00:00" endDate="2020-12-31T00:00:00"/>
     <bounds startDate="2019-01-01T00:00:00" endDate="2021-01-01T00:00:00"/>
   </state>
 </timelineCacheDefinition>
@@ -16123,7 +16123,7 @@
 
 <file path=xl/timelines/timeline1.xml><?xml version="1.0" encoding="utf-8"?>
 <timelines xmlns="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
-  <timeline name="Date" xr10:uid="{2951F72F-895B-4769-B806-7F047142FA4A}" cache="NativeTimeline_Date" caption="Date" level="2" selectionLevel="2" scrollPosition="2020-07-01T00:00:00"/>
+  <timeline name="Date" xr10:uid="{2951F72F-895B-4769-B806-7F047142FA4A}" cache="NativeTimeline_Date" caption="Date" level="2" selectionLevel="1" scrollPosition="2020-07-01T00:00:00"/>
 </timelines>
 </file>
 
@@ -16133,7 +16133,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -16260,14 +16260,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
-    <col min="2" max="2" width="18.69921875" customWidth="1"/>
-    <col min="3" max="3" width="33.796875" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" customWidth="1"/>
-    <col min="5" max="5" width="14.796875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.09765625" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -16309,25 +16309,25 @@
         <v>7</v>
       </c>
       <c r="B5" s="30">
-        <v>81522</v>
+        <v>99915</v>
       </c>
       <c r="C5" s="30">
-        <v>34414.25</v>
+        <v>46744.75</v>
       </c>
       <c r="D5" s="30">
-        <v>23228.799999999999</v>
+        <v>27795.599999999999</v>
       </c>
       <c r="E5" s="30">
-        <v>34902.5</v>
+        <v>36950</v>
       </c>
       <c r="F5" s="30">
-        <v>27520.5</v>
+        <v>29036</v>
       </c>
       <c r="G5" s="30">
-        <v>8657.5999999999985</v>
+        <v>10790.4</v>
       </c>
       <c r="H5" s="30">
-        <v>210245.65000000002</v>
+        <v>251231.75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -16335,25 +16335,25 @@
         <v>14</v>
       </c>
       <c r="B6" s="30">
-        <v>70356</v>
+        <v>86598</v>
       </c>
       <c r="C6" s="30">
-        <v>29061.5</v>
+        <v>36530</v>
       </c>
       <c r="D6" s="30">
-        <v>34554.799999999996</v>
+        <v>44136.400000000009</v>
       </c>
       <c r="E6" s="30">
         <v>33997.5</v>
       </c>
       <c r="F6" s="30">
-        <v>18305</v>
+        <v>25086.25</v>
       </c>
       <c r="G6" s="30">
-        <v>9571.2000000000007</v>
+        <v>10672</v>
       </c>
       <c r="H6" s="30">
-        <v>195846</v>
+        <v>237020.15000000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -16361,25 +16361,25 @@
         <v>17</v>
       </c>
       <c r="B7" s="30">
-        <v>67500</v>
+        <v>81960</v>
       </c>
       <c r="C7" s="30">
-        <v>43858.75</v>
+        <v>51853.75</v>
       </c>
       <c r="D7" s="30">
-        <v>32177.599999999999</v>
+        <v>41137.599999999999</v>
       </c>
       <c r="E7" s="30">
-        <v>14577.5</v>
+        <v>20900</v>
       </c>
       <c r="F7" s="30">
-        <v>27972</v>
+        <v>28736.75</v>
       </c>
       <c r="G7" s="30">
-        <v>8023.2</v>
+        <v>10924.8</v>
       </c>
       <c r="H7" s="30">
-        <v>194109.05</v>
+        <v>235512.9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -16387,25 +16387,25 @@
         <v>16</v>
       </c>
       <c r="B8" s="30">
-        <v>72831</v>
+        <v>80013</v>
       </c>
       <c r="C8" s="30">
-        <v>23029.5</v>
+        <v>27563.25</v>
       </c>
       <c r="D8" s="30">
-        <v>23083.200000000004</v>
+        <v>27795.600000000006</v>
       </c>
       <c r="E8" s="30">
-        <v>25822.5</v>
+        <v>27825</v>
       </c>
       <c r="F8" s="30">
-        <v>15384.25</v>
+        <v>16506</v>
       </c>
       <c r="G8" s="30">
-        <v>7951.9999999999991</v>
+        <v>9755.9999999999982</v>
       </c>
       <c r="H8" s="30">
-        <v>168102.45</v>
+        <v>189458.85</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -16413,25 +16413,25 @@
         <v>15</v>
       </c>
       <c r="B9" s="30">
-        <v>49086</v>
+        <v>60726</v>
       </c>
       <c r="C9" s="30">
-        <v>37719.5</v>
+        <v>41967.25</v>
       </c>
       <c r="D9" s="30">
-        <v>23615.199999999997</v>
+        <v>28335.999999999996</v>
       </c>
       <c r="E9" s="30">
-        <v>26897.5</v>
+        <v>33925</v>
       </c>
       <c r="F9" s="30">
-        <v>14320.25</v>
+        <v>15181.25</v>
       </c>
       <c r="G9" s="30">
-        <v>8628</v>
+        <v>9144</v>
       </c>
       <c r="H9" s="30">
-        <v>160266.45000000001</v>
+        <v>189279.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -16439,25 +16439,25 @@
         <v>22</v>
       </c>
       <c r="B10" s="30">
-        <v>341295</v>
+        <v>409212</v>
       </c>
       <c r="C10" s="30">
-        <v>168083.5</v>
+        <v>204659</v>
       </c>
       <c r="D10" s="30">
-        <v>136659.6</v>
+        <v>169201.2</v>
       </c>
       <c r="E10" s="30">
-        <v>136197.5</v>
+        <v>153597.5</v>
       </c>
       <c r="F10" s="30">
-        <v>103502</v>
+        <v>114546.25</v>
       </c>
       <c r="G10" s="30">
-        <v>42832</v>
+        <v>51287.199999999997</v>
       </c>
       <c r="H10" s="30">
-        <v>928569.60000000009</v>
+        <v>1102503.1499999999</v>
       </c>
     </row>
   </sheetData>
@@ -16477,8 +16477,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.8984375" customWidth="1"/>
     <col min="4" max="5" width="6.296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.69921875" bestFit="1" customWidth="1"/>
@@ -17624,8 +17624,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="13.09765625" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -17751,9 +17751,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G701"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33900,9 +33898,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G526"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:G526"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>